<commit_message>
Basic Renderer Stuff - Trying to Fix main
</commit_message>
<xml_diff>
--- a/Time Management.xlsx
+++ b/Time Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\University\Final Year Project\FinalYearProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A9A4BE-DEAC-47AF-8288-B7D4EC326FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EA66E6-3F03-45C5-9252-13D1EB5BCDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB3D7441-48F5-4337-9CEA-5ECCAD9F0A1E}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="128">
-  <si>
-    <t>1. Creating the SDL/Open GL Basic engine</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="132">
   <si>
     <t>1.1 Create a basic project linking SDL and Open GL together</t>
   </si>
@@ -420,6 +417,21 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Only works for square aspect ratios. Need to improve</t>
+  </si>
+  <si>
+    <t>Adjust speed and min max</t>
+  </si>
+  <si>
+    <t>Not tested with a sprite yet</t>
   </si>
 </sst>
 </file>
@@ -435,7 +447,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,12 +487,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -641,34 +647,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -712,6 +695,28 @@
       </fill>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -853,16 +858,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BA87E40-588D-49B5-AE0B-33DE123498D5}" name="Table4" displayName="Table4" ref="A1:E42" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:E42" xr:uid="{6BA87E40-588D-49B5-AE0B-33DE123498D5}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BA87E40-588D-49B5-AE0B-33DE123498D5}" name="Table4" displayName="Table4" ref="A1:F42" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:F42" xr:uid="{6BA87E40-588D-49B5-AE0B-33DE123498D5}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{09DD4744-8278-4B76-B58F-AEF0A75FFAAA}" name="Task" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{0C506CD1-72AB-412B-9B87-FC5E42CE04AF}" name="Total Days" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{09C2A5A7-4AFB-42EB-86E6-515A127536C2}" name="Dev Days" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{9745CF59-685B-4247-8274-8AAAF83C0AB9}" name="Test Days" dataDxfId="7">
       <calculatedColumnFormula xml:space="preserve"> B2-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0D5201E8-3987-4C75-AA70-55F254369150}" name="Status" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{0D5201E8-3987-4C75-AA70-55F254369150}" name="Status" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{59973D58-3C1E-4F57-B6BD-0011552E538D}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1168,7 +1174,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1178,28 +1184,32 @@
     <col min="3" max="3" width="12.6328125" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" customWidth="1"/>
     <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="B2" s="7">
         <f>SUM(B3:B9)</f>
@@ -1218,7 +1228,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
@@ -1235,7 +1245,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
@@ -1248,10 +1258,13 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="22"/>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -1263,11 +1276,11 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
@@ -1279,11 +1292,11 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
@@ -1296,10 +1309,13 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="22"/>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7">
         <v>2</v>
@@ -1312,10 +1328,13 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="22"/>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7">
         <v>3</v>
@@ -1327,11 +1346,11 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E9" s="24"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="7">
         <f>SUM(B11:B15)</f>
@@ -1349,7 +1368,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="7">
         <v>4</v>
@@ -1365,7 +1384,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="7">
         <v>3</v>
@@ -1381,7 +1400,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="7">
         <v>3</v>
@@ -1397,7 +1416,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7">
         <v>5</v>
@@ -1413,7 +1432,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="7">
         <v>2</v>
@@ -1429,7 +1448,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7">
         <f>SUM(B17:B18)</f>
@@ -1447,7 +1466,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="7">
         <v>5</v>
@@ -1463,7 +1482,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="7">
         <v>5</v>
@@ -1479,7 +1498,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="7">
         <f>SUM(B20:B28)</f>
@@ -1497,7 +1516,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="7">
         <v>2</v>
@@ -1513,7 +1532,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="7">
         <v>5</v>
@@ -1529,7 +1548,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="7">
         <v>1</v>
@@ -1545,7 +1564,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="7">
         <v>7</v>
@@ -1561,7 +1580,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="7">
         <v>7</v>
@@ -1577,7 +1596,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="7">
         <v>7</v>
@@ -1593,7 +1612,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="7">
         <v>12</v>
@@ -1609,7 +1628,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="7">
         <v>2</v>
@@ -1625,7 +1644,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="7">
         <v>4</v>
@@ -1641,7 +1660,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="7">
         <f>SUM(B30:B31)</f>
@@ -1659,7 +1678,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="7">
         <v>2</v>
@@ -1675,7 +1694,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="7">
         <v>3</v>
@@ -1691,7 +1710,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="7">
         <f>SUM(B33:B36)</f>
@@ -1709,7 +1728,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="7">
         <v>10</v>
@@ -1725,7 +1744,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="7">
         <v>13</v>
@@ -1741,7 +1760,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="7">
         <v>5</v>
@@ -1757,7 +1776,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="7">
         <v>25</v>
@@ -1773,7 +1792,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="7">
         <f>SUM(B38:B42)</f>
@@ -1791,7 +1810,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="7">
         <v>0</v>
@@ -1807,7 +1826,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="7">
         <v>0</v>
@@ -1823,7 +1842,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="7">
         <v>0</v>
@@ -1839,7 +1858,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="7">
         <v>0</v>
@@ -1855,7 +1874,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="10">
         <v>0</v>
@@ -1871,7 +1890,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2">
         <f>SUM(B2,B10,B16,B19,B29,B32,B37)</f>
@@ -1880,7 +1899,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" s="2">
         <f>SUM(C2,C10,C16,C19,C29,C32,C37)</f>
@@ -1889,7 +1908,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" s="2">
         <f>SUM(D2,D10,D16,D19,D29,D32,D37)</f>
@@ -1898,7 +1917,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="2">
         <f xml:space="preserve"> 178-B44</f>
@@ -1935,30 +1954,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1971,18 +1990,18 @@
         <v>3.5</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -1995,18 +2014,18 @@
         <v>3.5</v>
       </c>
       <c r="E3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>58</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -2019,18 +2038,18 @@
         <v>4</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="G4" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="9">
         <v>2</v>
@@ -2043,18 +2062,18 @@
         <v>2</v>
       </c>
       <c r="E5" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9">
         <v>2.5</v>
@@ -2067,18 +2086,18 @@
         <v>3.75</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="9">
         <v>2.5</v>
@@ -2091,18 +2110,18 @@
         <v>3.75</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="G7" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9">
         <v>3</v>
@@ -2115,18 +2134,18 @@
         <v>4.5</v>
       </c>
       <c r="E8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>70</v>
-      </c>
       <c r="G8" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="9">
         <v>3</v>
@@ -2139,18 +2158,18 @@
         <v>15</v>
       </c>
       <c r="E9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="9">
         <v>4</v>
@@ -2163,18 +2182,18 @@
         <v>20</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="9">
         <v>2</v>
@@ -2187,18 +2206,18 @@
         <v>10</v>
       </c>
       <c r="E11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="G11" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="9">
         <v>4</v>
@@ -2211,18 +2230,18 @@
         <v>8</v>
       </c>
       <c r="E12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="G12" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="9">
         <v>4</v>
@@ -2235,18 +2254,18 @@
         <v>8</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="9">
         <v>3.5</v>
@@ -2259,18 +2278,18 @@
         <v>12.25</v>
       </c>
       <c r="E14" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="G14" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="9">
         <v>3</v>
@@ -2283,18 +2302,18 @@
         <v>6</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9">
         <v>2.5</v>
@@ -2307,18 +2326,18 @@
         <v>12.5</v>
       </c>
       <c r="E16" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>87</v>
-      </c>
       <c r="G16" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9">
         <v>3.5</v>
@@ -2331,18 +2350,18 @@
         <v>17.5</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
@@ -2355,18 +2374,18 @@
         <v>4</v>
       </c>
       <c r="E18" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="G18" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="9">
         <v>4</v>
@@ -2379,18 +2398,18 @@
         <v>14</v>
       </c>
       <c r="E19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="G19" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="9">
         <v>3</v>
@@ -2403,18 +2422,18 @@
         <v>9</v>
       </c>
       <c r="E20" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="G20" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="9">
         <v>5</v>
@@ -2427,18 +2446,18 @@
         <v>17.5</v>
       </c>
       <c r="E21" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="G21" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="9">
         <v>4</v>
@@ -2451,18 +2470,18 @@
         <v>14</v>
       </c>
       <c r="E22" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="G22" s="18" t="s">
         <v>102</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="9">
         <v>2.5</v>
@@ -2475,18 +2494,18 @@
         <v>2.5</v>
       </c>
       <c r="E23" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="G23" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -2499,18 +2518,18 @@
         <v>1</v>
       </c>
       <c r="E24" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="G24" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="9">
         <v>1.5</v>
@@ -2523,18 +2542,18 @@
         <v>3.75</v>
       </c>
       <c r="E25" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="G25" s="18" t="s">
         <v>111</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="9">
         <v>1.5</v>
@@ -2547,18 +2566,18 @@
         <v>4.5</v>
       </c>
       <c r="E26" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="G26" s="18" t="s">
         <v>114</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="9">
         <v>3</v>
@@ -2571,18 +2590,18 @@
         <v>15</v>
       </c>
       <c r="E27" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="G27" s="18" t="s">
         <v>117</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="9">
         <v>3</v>
@@ -2595,18 +2614,18 @@
         <v>15</v>
       </c>
       <c r="E28" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F28" s="18" t="s">
-        <v>120</v>
-      </c>
       <c r="G28" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="9">
         <v>2</v>
@@ -2619,18 +2638,18 @@
         <v>8</v>
       </c>
       <c r="E29" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="18" t="s">
-        <v>122</v>
-      </c>
       <c r="G29" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="9">
         <v>4</v>
@@ -2643,98 +2662,98 @@
         <v>20</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="19"/>
       <c r="E31" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="19"/>
       <c r="E32" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="19"/>
       <c r="E33" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="19"/>
       <c r="E34" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="19"/>
       <c r="E35" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -2743,33 +2762,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>4.1</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D35 D107:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>0</formula>
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>9</formula>
       <formula>17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>17</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>